<commit_message>
Under 1 second implementation
This code is under 1 second for a 1024 x 1024 hologram generation. Needs to be refactored
</commit_message>
<xml_diff>
--- a/version2 code/python results- version1.xlsx
+++ b/version2 code/python results- version1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wits\fourth year\lab project\Code\Py Code\LabProject\version2 code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Wits\Lab project\Code\Test code\Py Code\LabProject\version2 code\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -213,6 +213,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -248,6 +265,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">

</xml_diff>